<commit_message>
RuleManager - Add reponse protocol
</commit_message>
<xml_diff>
--- a/doc/Docs/protocol_0623.xlsx
+++ b/doc/Docs/protocol_0623.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="27735" windowHeight="7875" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="27735" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="protocol" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="214">
   <si>
     <t>Rule</t>
   </si>
@@ -780,6 +780,50 @@
   </si>
   <si>
     <t>Module</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RuleManager</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Targets</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RuleCtrl</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{errorString}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Success/Fail}</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -878,7 +922,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1380,11 +1424,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1403,16 +1458,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1422,15 +1471,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1440,18 +1480,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1463,36 +1491,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1505,46 +1509,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1569,25 +1537,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1632,6 +1582,120 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1935,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM551"/>
+  <dimension ref="A1:AM555"/>
   <sheetViews>
-    <sheetView topLeftCell="G49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1992,31 +2056,31 @@
     </row>
     <row r="2" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="39" t="s">
         <v>45</v>
       </c>
       <c r="K2" s="4"/>
@@ -2051,31 +2115,31 @@
     </row>
     <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="10">
+      <c r="B3" s="72">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="17" t="s">
         <v>153</v>
       </c>
       <c r="K3" s="4"/>
@@ -2110,19 +2174,19 @@
     </row>
     <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="20" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="17" t="s">
         <v>155</v>
       </c>
       <c r="K4" s="4"/>
@@ -2157,19 +2221,19 @@
     </row>
     <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="14" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="J5" s="16"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2202,27 +2266,27 @@
     </row>
     <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="19" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="17" t="s">
         <v>153</v>
       </c>
       <c r="K6" s="4"/>
@@ -2257,19 +2321,19 @@
     </row>
     <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="23" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="86" t="s">
+      <c r="J7" s="51" t="s">
         <v>162</v>
       </c>
       <c r="K7" s="4"/>
@@ -2304,19 +2368,19 @@
     </row>
     <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -2349,19 +2413,19 @@
     </row>
     <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="22"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -2394,19 +2458,19 @@
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -2439,19 +2503,19 @@
     </row>
     <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20" t="s">
+      <c r="B11" s="73"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="22"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -2484,19 +2548,19 @@
     </row>
     <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20" t="s">
+      <c r="B12" s="73"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="22"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -2529,19 +2593,19 @@
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20" t="s">
+      <c r="B13" s="73"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="22"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -2574,19 +2638,19 @@
     </row>
     <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -2619,19 +2683,19 @@
     </row>
     <row r="15" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -2664,31 +2728,31 @@
     </row>
     <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="13">
+      <c r="B16" s="73">
         <v>2</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="17" t="s">
         <v>154</v>
       </c>
       <c r="K16" s="4"/>
@@ -2723,19 +2787,19 @@
     </row>
     <row r="17" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="23" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="J17" s="86" t="s">
+      <c r="J17" s="51" t="s">
         <v>152</v>
       </c>
       <c r="K17" s="4"/>
@@ -2770,19 +2834,19 @@
     </row>
     <row r="18" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="20" t="s">
+      <c r="B18" s="73"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="22"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -2815,19 +2879,19 @@
     </row>
     <row r="19" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="20" t="s">
+      <c r="B19" s="73"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="J19" s="22"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -2860,19 +2924,19 @@
     </row>
     <row r="20" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="20" t="s">
+      <c r="B20" s="73"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="J20" s="22"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -2905,19 +2969,19 @@
     </row>
     <row r="21" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="69" t="s">
+      <c r="B21" s="73"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="J21" s="16"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -2950,27 +3014,27 @@
     </row>
     <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="73" t="s">
+      <c r="B22" s="73"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="75" t="s">
+      <c r="E22" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="75" t="s">
+      <c r="F22" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="17" t="s">
         <v>154</v>
       </c>
       <c r="K22" s="4"/>
@@ -3005,19 +3069,19 @@
     </row>
     <row r="23" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="23" t="s">
+      <c r="B23" s="73"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="I23" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="17" t="s">
         <v>163</v>
       </c>
       <c r="K23" s="4"/>
@@ -3052,19 +3116,19 @@
     </row>
     <row r="24" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="20" t="s">
+      <c r="B24" s="73"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="J24" s="22"/>
+      <c r="J24" s="17"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -3097,19 +3161,19 @@
     </row>
     <row r="25" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="20" t="s">
+      <c r="B25" s="73"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J25" s="22"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -3142,19 +3206,19 @@
     </row>
     <row r="26" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="20" t="s">
+      <c r="B26" s="73"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="J26" s="78" t="s">
+      <c r="J26" s="43" t="s">
         <v>142</v>
       </c>
       <c r="K26" s="4"/>
@@ -3189,31 +3253,31 @@
     </row>
     <row r="27" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="10">
+      <c r="B27" s="72">
         <v>3</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I27" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="17" t="s">
         <v>154</v>
       </c>
       <c r="K27" s="4"/>
@@ -3248,19 +3312,19 @@
     </row>
     <row r="28" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20" t="s">
+      <c r="B28" s="73"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="17" t="s">
         <v>161</v>
       </c>
       <c r="K28" s="4"/>
@@ -3295,19 +3359,19 @@
     </row>
     <row r="29" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20" t="s">
+      <c r="B29" s="73"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="21" t="s">
+      <c r="I29" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J29" s="22"/>
+      <c r="J29" s="17"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -3340,19 +3404,19 @@
     </row>
     <row r="30" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20" t="s">
+      <c r="B30" s="73"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="J30" s="22"/>
+      <c r="J30" s="17"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -3385,19 +3449,19 @@
     </row>
     <row r="31" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20" t="s">
+      <c r="B31" s="73"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="21" t="s">
+      <c r="I31" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="J31" s="22"/>
+      <c r="J31" s="17"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -3430,19 +3494,19 @@
     </row>
     <row r="32" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28" t="s">
+      <c r="B32" s="84"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="29" t="s">
+      <c r="I32" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="J32" s="30" t="s">
+      <c r="J32" s="21" t="s">
         <v>143</v>
       </c>
       <c r="K32" s="4"/>
@@ -3477,900 +3541,926 @@
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="13">
+      <c r="B33" s="73">
         <v>4</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H33" s="44" t="s">
+      <c r="H33" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="I33" s="45" t="s">
+      <c r="I33" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="J33" s="22" t="s">
+      <c r="J33" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="44" t="s">
+      <c r="B34" s="73"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="45" t="s">
+      <c r="I34" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="J34" s="17" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="44" t="s">
+      <c r="B35" s="73"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="I35" s="45" t="s">
+      <c r="I35" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="J35" s="22"/>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="46" t="s">
+      <c r="B36" s="73"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="I36" s="47" t="s">
+      <c r="I36" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="22"/>
+      <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="46" t="s">
+      <c r="B37" s="73"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I37" s="21" t="s">
+      <c r="I37" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J37" s="22"/>
+      <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="46" t="s">
+      <c r="B38" s="73"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I38" s="21" t="s">
+      <c r="I38" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J38" s="78" t="s">
+      <c r="J38" s="43" t="s">
         <v>144</v>
       </c>
       <c r="AF38" s="4"/>
     </row>
     <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="10">
+      <c r="B39" s="72">
         <v>5</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F39" s="33" t="s">
+      <c r="F39" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I39" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J39" s="22" t="s">
+      <c r="J39" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="44" t="s">
+      <c r="B40" s="73"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="45" t="s">
+      <c r="I40" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="22" t="s">
+      <c r="J40" s="17" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="44" t="s">
+      <c r="B41" s="73"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="J41" s="22"/>
+      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="44" t="s">
+      <c r="B42" s="73"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="I42" s="45" t="s">
+      <c r="I42" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J42" s="22"/>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="44" t="s">
+      <c r="B43" s="73"/>
+      <c r="C43" s="82"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I43" s="21" t="s">
+      <c r="I43" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J43" s="22"/>
+      <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="49" t="s">
+      <c r="B44" s="73"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="J44" s="16"/>
+      <c r="J44" s="14"/>
     </row>
     <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="19" t="s">
+      <c r="B45" s="73"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I45" s="21" t="s">
+      <c r="I45" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J45" s="22" t="s">
+      <c r="J45" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="44" t="s">
+      <c r="B46" s="73"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="I46" s="45" t="s">
+      <c r="I46" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J46" s="22" t="s">
+      <c r="J46" s="17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="44" t="s">
+      <c r="B47" s="73"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="I47" s="45" t="s">
+      <c r="I47" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="22"/>
+      <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="44" t="s">
+      <c r="B48" s="73"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="I48" s="45" t="s">
+      <c r="I48" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J48" s="22"/>
+      <c r="J48" s="17"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="44" t="s">
+      <c r="B49" s="73"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="I49" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J49" s="22"/>
+      <c r="J49" s="17"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="50" t="s">
+      <c r="B50" s="84"/>
+      <c r="C50" s="83"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="79"/>
+      <c r="H50" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="I50" s="28" t="s">
+      <c r="I50" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J50" s="30"/>
+      <c r="J50" s="21"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="B51" s="10">
+      <c r="B51" s="72">
         <v>6</v>
       </c>
-      <c r="C51" s="41" t="s">
+      <c r="C51" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="33" t="s">
+      <c r="F51" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G51" s="34" t="s">
+      <c r="G51" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H51" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I51" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J51" s="22" t="s">
+      <c r="J51" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20" t="s">
+      <c r="B52" s="73"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="64"/>
+      <c r="H52" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="21" t="s">
+      <c r="I52" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="J52" s="22" t="s">
+      <c r="J52" s="17" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20" t="s">
+      <c r="B53" s="73"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="64"/>
+      <c r="H53" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="21" t="s">
+      <c r="I53" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="J53" s="22" t="s">
+      <c r="J53" s="17" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="20" t="s">
+      <c r="B54" s="73"/>
+      <c r="C54" s="82"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="I54" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J54" s="22" t="s">
+      <c r="J54" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="14" t="s">
+      <c r="B55" s="73"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="65"/>
+      <c r="H55" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I55" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J55" s="38"/>
+      <c r="J55" s="24"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="H56" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="21" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="F56" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="G56" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="H56" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="I56" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="J56" s="22" t="s">
+      <c r="J56" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I57" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="J57" s="39" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I57" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="J57" s="25"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="I58" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J58" s="40"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="64"/>
+      <c r="H58" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="I58" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="13">
+      <c r="B59" s="73"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="J59" s="24"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="73"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="G60" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="67"/>
+      <c r="H61" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I61" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J61" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="84"/>
+      <c r="C62" s="83"/>
+      <c r="D62" s="79"/>
+      <c r="E62" s="80"/>
+      <c r="F62" s="78"/>
+      <c r="G62" s="79"/>
+      <c r="H62" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I62" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J62" s="26"/>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="73">
         <v>7</v>
       </c>
-      <c r="C59" s="42" t="s">
+      <c r="C63" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D63" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E63" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F63" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G63" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="H59" s="20" t="s">
+      <c r="H63" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I59" s="21" t="s">
+      <c r="I63" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="J59" s="22" t="s">
+      <c r="J63" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="20" t="s">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="70"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="67"/>
+      <c r="H64" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I60" s="21" t="s">
+      <c r="I64" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="J60" s="22" t="s">
+      <c r="J64" s="17" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="20" t="s">
+    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="82"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="70"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="67"/>
+      <c r="H65" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I61" s="21" t="s">
+      <c r="I65" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="J61" s="39"/>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="20" t="s">
+      <c r="J65" s="25"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="67"/>
+      <c r="H66" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="21" t="s">
+      <c r="I66" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J62" s="77" t="s">
+      <c r="J66" s="42" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="51">
+    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="88">
         <v>8</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C67" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="53" t="s">
+      <c r="D67" s="90" t="s">
         <v>117</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E67" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="33" t="s">
+      <c r="F67" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="34" t="s">
+      <c r="G67" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="H63" s="11" t="s">
+      <c r="H67" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="12" t="s">
+      <c r="I67" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J63" s="22" t="s">
+      <c r="J67" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="55"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="20" t="s">
+    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="87"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="67"/>
+      <c r="H68" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I64" s="21" t="s">
+      <c r="I68" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="J64" s="22" t="s">
+      <c r="J68" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="57"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="28" t="s">
+    <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="89"/>
+      <c r="C69" s="93"/>
+      <c r="D69" s="91"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="I65" s="29" t="s">
+      <c r="I69" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="40" t="s">
+      <c r="J69" s="26" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="54">
+    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="87">
         <v>9</v>
       </c>
-      <c r="C66" s="55" t="s">
+      <c r="C70" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="D66" s="56" t="s">
+      <c r="D70" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="E66" s="17" t="s">
+      <c r="E70" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="F66" s="18" t="s">
+      <c r="F70" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="G70" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="H66" s="20" t="s">
+      <c r="H70" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I66" s="21" t="s">
+      <c r="I70" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J66" s="22" t="s">
+      <c r="J70" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="54"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="20" t="s">
+    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="85"/>
+      <c r="E71" s="70"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="67"/>
+      <c r="H71" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I67" s="21" t="s">
+      <c r="I71" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J67" s="22" t="s">
+      <c r="J71" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="54"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="I68" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J68" s="77"/>
-    </row>
-    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="51">
-        <v>10</v>
-      </c>
-      <c r="C69" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="E69" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="G69" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J69" s="22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="B70" s="54"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I70" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J70" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="54"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I71" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J71" s="39"/>
     </row>
     <row r="72" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
-      <c r="B72" s="57"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="28" t="s">
+      <c r="B72" s="87"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="85"/>
+      <c r="E72" s="70"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="67"/>
+      <c r="H72" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I72" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="J72" s="30"/>
+      <c r="I72" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" s="42"/>
     </row>
     <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="52">
+      <c r="B73" s="88">
+        <v>10</v>
+      </c>
+      <c r="C73" s="92" t="s">
+        <v>124</v>
+      </c>
+      <c r="D73" s="90" t="s">
+        <v>117</v>
+      </c>
+      <c r="E73" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="H73" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="52" t="s">
+      <c r="I73" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="85"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="67"/>
+      <c r="H74" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J74" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="85"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="67"/>
+      <c r="H75" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I75" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J75" s="25"/>
+    </row>
+    <row r="76" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+      <c r="B76" s="89"/>
+      <c r="C76" s="93"/>
+      <c r="D76" s="91"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="78"/>
+      <c r="G76" s="79"/>
+      <c r="H76" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="J76" s="21"/>
+    </row>
+    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="92">
+        <v>11</v>
+      </c>
+      <c r="C77" s="92" t="s">
         <v>126</v>
       </c>
-      <c r="D73" s="60" t="s">
+      <c r="D77" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="E73" s="33" t="s">
+      <c r="E77" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="F73" s="33" t="s">
+      <c r="F77" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="G73" s="33" t="s">
+      <c r="G77" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="H73" s="20" t="s">
+      <c r="H77" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I73" s="21" t="s">
+      <c r="I77" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="J73" s="22" t="s">
+      <c r="J77" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="20" t="s">
+    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="86"/>
+      <c r="C78" s="86"/>
+      <c r="D78" s="95"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="64"/>
+      <c r="H78" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="21"/>
-      <c r="J74" s="22"/>
-    </row>
-    <row r="75" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
-      <c r="B75" s="58"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="28" t="s">
+      <c r="I78" s="16"/>
+      <c r="J78" s="17"/>
+    </row>
+    <row r="79" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4"/>
+      <c r="B79" s="93"/>
+      <c r="C79" s="93"/>
+      <c r="D79" s="96"/>
+      <c r="E79" s="78"/>
+      <c r="F79" s="78"/>
+      <c r="G79" s="78"/>
+      <c r="H79" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I75" s="28" t="s">
+      <c r="I79" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="J75" s="30" t="s">
+      <c r="J79" s="21" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="3"/>
-    </row>
-    <row r="77" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="5"/>
-    </row>
-    <row r="78" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="5"/>
     </row>
     <row r="80" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
@@ -4382,7 +4472,7 @@
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
-      <c r="J80" s="5"/>
+      <c r="J80" s="3"/>
     </row>
     <row r="81" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
@@ -4394,19 +4484,19 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
-      <c r="J81" s="3"/>
+      <c r="J81" s="5"/>
     </row>
     <row r="82" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
-      <c r="J82" s="3"/>
+      <c r="J82" s="5"/>
     </row>
     <row r="83" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
@@ -4422,9 +4512,9 @@
     </row>
     <row r="84" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
@@ -4445,7 +4535,7 @@
       <c r="J85" s="3"/>
     </row>
     <row r="86" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
+      <c r="A86" s="4"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -4465,14 +4555,14 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
-      <c r="I87" s="7"/>
+      <c r="I87" s="6"/>
       <c r="J87" s="5"/>
     </row>
     <row r="88" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -4490,10 +4580,10 @@
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
-      <c r="J89" s="5"/>
+      <c r="J89" s="3"/>
     </row>
     <row r="90" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
+      <c r="A90" s="2"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -4502,7 +4592,7 @@
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="5"/>
+      <c r="J90" s="3"/>
     </row>
     <row r="91" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
@@ -4513,23 +4603,23 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="3"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="5"/>
     </row>
     <row r="92" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
-      <c r="J92" s="3"/>
+      <c r="J92" s="5"/>
     </row>
     <row r="93" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
+      <c r="A93" s="4"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -4541,7 +4631,7 @@
       <c r="J93" s="5"/>
     </row>
     <row r="94" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
+      <c r="A94" s="4"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -4565,10 +4655,10 @@
       <c r="J95" s="3"/>
     </row>
     <row r="96" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="A96" s="2"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -4577,7 +4667,7 @@
       <c r="J96" s="3"/>
     </row>
     <row r="97" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
+      <c r="A97" s="2"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -4590,9 +4680,9 @@
     </row>
     <row r="98" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -4602,21 +4692,21 @@
     </row>
     <row r="99" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
-      <c r="J99" s="5"/>
+      <c r="J99" s="3"/>
     </row>
     <row r="100" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
       <c r="E100" s="6"/>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
@@ -4634,13 +4724,13 @@
       <c r="G101" s="6"/>
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
-      <c r="J101" s="3"/>
+      <c r="J101" s="5"/>
     </row>
     <row r="102" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
@@ -4650,9 +4740,9 @@
     </row>
     <row r="103" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="7"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
       <c r="E103" s="6"/>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
@@ -4661,7 +4751,7 @@
       <c r="J103" s="5"/>
     </row>
     <row r="104" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
+      <c r="A104" s="2"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
@@ -4670,7 +4760,7 @@
       <c r="G104" s="6"/>
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="5"/>
+      <c r="J104" s="3"/>
     </row>
     <row r="105" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
@@ -4682,22 +4772,22 @@
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
       <c r="I105" s="6"/>
-      <c r="J105" s="5"/>
+      <c r="J105" s="3"/>
     </row>
     <row r="106" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
       <c r="E106" s="6"/>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
       <c r="H106" s="6"/>
       <c r="I106" s="6"/>
-      <c r="J106" s="3"/>
+      <c r="J106" s="5"/>
     </row>
     <row r="107" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A107" s="2"/>
+      <c r="A107" s="4"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -4709,19 +4799,19 @@
       <c r="J107" s="5"/>
     </row>
     <row r="108" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A108" s="2"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
       <c r="H108" s="6"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="3"/>
+      <c r="J108" s="5"/>
     </row>
     <row r="109" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A109" s="2"/>
+      <c r="A109" s="4"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -4733,16 +4823,16 @@
       <c r="J109" s="5"/>
     </row>
     <row r="110" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A110" s="2"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
-      <c r="J110" s="5"/>
+      <c r="J110" s="3"/>
     </row>
     <row r="111" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
@@ -4766,55 +4856,55 @@
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
-      <c r="J112" s="5"/>
-    </row>
-    <row r="113" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J112" s="3"/>
+    </row>
+    <row r="113" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
-      <c r="I113" s="8"/>
-      <c r="J113" s="2"/>
-    </row>
-    <row r="114" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
-      <c r="I114" s="8"/>
-      <c r="J114" s="2"/>
-    </row>
-    <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
-      <c r="I115" s="8"/>
-      <c r="J115" s="2"/>
-    </row>
-    <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
-      <c r="I116" s="8"/>
-      <c r="J116" s="2"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="5"/>
     </row>
     <row r="117" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
@@ -4862,54 +4952,54 @@
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
-      <c r="J120" s="4"/>
+      <c r="J120" s="2"/>
     </row>
     <row r="121" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
-      <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-      <c r="H121" s="7"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
       <c r="I121" s="8"/>
-      <c r="J121" s="4"/>
+      <c r="J121" s="2"/>
     </row>
     <row r="122" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-      <c r="H122" s="7"/>
-      <c r="I122" s="7"/>
-      <c r="J122" s="4"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="2"/>
     </row>
     <row r="123" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
-      <c r="H123" s="7"/>
-      <c r="I123" s="7"/>
-      <c r="J123" s="4"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="2"/>
     </row>
     <row r="124" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-      <c r="G124" s="7"/>
-      <c r="H124" s="7"/>
-      <c r="I124" s="7"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
       <c r="J124" s="4"/>
     </row>
     <row r="125" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4921,7 +5011,7 @@
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
-      <c r="I125" s="7"/>
+      <c r="I125" s="8"/>
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4953,10 +5043,10 @@
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
-      <c r="E128" s="9"/>
-      <c r="F128" s="9"/>
-      <c r="G128" s="9"/>
-      <c r="H128" s="8"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
+      <c r="G128" s="7"/>
+      <c r="H128" s="7"/>
       <c r="I128" s="7"/>
       <c r="J128" s="4"/>
     </row>
@@ -4965,11 +5055,11 @@
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-      <c r="I129" s="8"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="7"/>
+      <c r="H129" s="7"/>
+      <c r="I129" s="7"/>
       <c r="J129" s="4"/>
     </row>
     <row r="130" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4977,11 +5067,11 @@
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="7"/>
+      <c r="H130" s="7"/>
+      <c r="I130" s="7"/>
       <c r="J130" s="4"/>
     </row>
     <row r="131" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4989,11 +5079,11 @@
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
+      <c r="G131" s="7"/>
+      <c r="H131" s="7"/>
+      <c r="I131" s="7"/>
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5001,11 +5091,11 @@
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
-      <c r="E132" s="8"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
       <c r="H132" s="8"/>
-      <c r="I132" s="8"/>
+      <c r="I132" s="7"/>
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5029,7 +5119,7 @@
       <c r="F134" s="8"/>
       <c r="G134" s="8"/>
       <c r="H134" s="8"/>
-      <c r="I134" s="7"/>
+      <c r="I134" s="8"/>
       <c r="J134" s="4"/>
     </row>
     <row r="135" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5037,11 +5127,11 @@
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
-      <c r="E135" s="9"/>
-      <c r="F135" s="9"/>
-      <c r="G135" s="9"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
       <c r="H135" s="8"/>
-      <c r="I135" s="7"/>
+      <c r="I135" s="8"/>
       <c r="J135" s="4"/>
     </row>
     <row r="136" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5069,7 +5159,7 @@
       <c r="J137" s="4"/>
     </row>
     <row r="138" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A138" s="4"/>
+      <c r="A138" s="2"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
@@ -5077,23 +5167,23 @@
       <c r="F138" s="8"/>
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
-      <c r="I138" s="8"/>
+      <c r="I138" s="7"/>
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A139" s="4"/>
+      <c r="A139" s="2"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
       <c r="H139" s="8"/>
-      <c r="I139" s="8"/>
+      <c r="I139" s="7"/>
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A140" s="4"/>
+      <c r="A140" s="2"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
@@ -5101,7 +5191,7 @@
       <c r="F140" s="8"/>
       <c r="G140" s="8"/>
       <c r="H140" s="8"/>
-      <c r="I140" s="7"/>
+      <c r="I140" s="8"/>
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5113,7 +5203,7 @@
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
       <c r="H141" s="8"/>
-      <c r="I141" s="7"/>
+      <c r="I141" s="8"/>
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -5125,26 +5215,26 @@
       <c r="F142" s="8"/>
       <c r="G142" s="8"/>
       <c r="H142" s="8"/>
-      <c r="I142" s="7"/>
+      <c r="I142" s="8"/>
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A143" s="2"/>
+      <c r="A143" s="4"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
-      <c r="E143" s="9"/>
-      <c r="F143" s="9"/>
-      <c r="G143" s="9"/>
-      <c r="H143" s="7"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
       <c r="I143" s="8"/>
       <c r="J143" s="4"/>
     </row>
     <row r="144" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A144" s="2"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
+      <c r="A144" s="4"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
       <c r="G144" s="8"/>
@@ -5154,77 +5244,77 @@
     </row>
     <row r="145" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
       <c r="G145" s="8"/>
       <c r="H145" s="8"/>
-      <c r="I145" s="8"/>
+      <c r="I145" s="7"/>
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A146" s="2"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
+      <c r="A146" s="4"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
       <c r="G146" s="8"/>
       <c r="H146" s="8"/>
-      <c r="I146" s="8"/>
+      <c r="I146" s="7"/>
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A147" s="4"/>
+      <c r="A147" s="2"/>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8"/>
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="7"/>
       <c r="I147" s="8"/>
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A148" s="4"/>
+      <c r="A148" s="2"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7"/>
-      <c r="G148" s="7"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
       <c r="H148" s="8"/>
       <c r="I148" s="7"/>
       <c r="J148" s="4"/>
     </row>
     <row r="149" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A149" s="4"/>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
-      <c r="G149" s="7"/>
+      <c r="A149" s="2"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="8"/>
+      <c r="F149" s="8"/>
+      <c r="G149" s="8"/>
       <c r="H149" s="8"/>
-      <c r="I149" s="7"/>
+      <c r="I149" s="8"/>
       <c r="J149" s="4"/>
     </row>
     <row r="150" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
-      <c r="I150" s="7"/>
+      <c r="I150" s="8"/>
       <c r="J150" s="4"/>
     </row>
-    <row r="151" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
@@ -5234,58 +5324,58 @@
       <c r="G151" s="8"/>
       <c r="H151" s="8"/>
       <c r="I151" s="8"/>
-      <c r="J151" s="2"/>
+      <c r="J151" s="4"/>
     </row>
     <row r="152" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A152" s="2"/>
-      <c r="B152" s="8"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
+      <c r="A152" s="4"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
       <c r="E152" s="7"/>
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
-      <c r="H152" s="7"/>
+      <c r="H152" s="8"/>
       <c r="I152" s="7"/>
-      <c r="J152" s="2"/>
-    </row>
-    <row r="153" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J152" s="4"/>
+    </row>
+    <row r="153" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-      <c r="D153" s="7"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
-      <c r="H153" s="7"/>
+      <c r="H153" s="8"/>
       <c r="I153" s="7"/>
-      <c r="J153" s="2"/>
+      <c r="J153" s="4"/>
     </row>
     <row r="154" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-      <c r="H154" s="7"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
       <c r="I154" s="7"/>
-      <c r="J154" s="2"/>
-    </row>
-    <row r="155" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J154" s="4"/>
+    </row>
+    <row r="155" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-      <c r="H155" s="7"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="8"/>
+      <c r="F155" s="8"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="8"/>
       <c r="I155" s="8"/>
-      <c r="J155" s="4"/>
+      <c r="J155" s="2"/>
     </row>
     <row r="156" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A156" s="4"/>
+      <c r="A156" s="2"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
@@ -5293,10 +5383,10 @@
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
       <c r="H156" s="7"/>
-      <c r="I156" s="8"/>
-      <c r="J156" s="4"/>
-    </row>
-    <row r="157" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I156" s="7"/>
+      <c r="J156" s="2"/>
+    </row>
+    <row r="157" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -5306,19 +5396,19 @@
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-      <c r="J157" s="4"/>
+      <c r="J157" s="2"/>
     </row>
     <row r="158" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A158" s="4"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="E158" s="8"/>
-      <c r="F158" s="8"/>
-      <c r="G158" s="8"/>
+      <c r="A158" s="2"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="7"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+      <c r="F158" s="7"/>
+      <c r="G158" s="7"/>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-      <c r="J158" s="4"/>
+      <c r="J158" s="2"/>
     </row>
     <row r="159" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
@@ -5329,11 +5419,11 @@
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
       <c r="H159" s="7"/>
-      <c r="I159" s="7"/>
+      <c r="I159" s="8"/>
       <c r="J159" s="4"/>
     </row>
     <row r="160" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A160" s="2"/>
+      <c r="A160" s="4"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
@@ -5341,55 +5431,55 @@
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
-      <c r="I160" s="7"/>
+      <c r="I160" s="8"/>
       <c r="J160" s="4"/>
     </row>
-    <row r="161" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="4"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
-      <c r="E161" s="8"/>
-      <c r="F161" s="8"/>
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
+      <c r="G161" s="7"/>
+      <c r="H161" s="7"/>
       <c r="I161" s="7"/>
       <c r="J161" s="4"/>
     </row>
-    <row r="162" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="4"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
       <c r="E162" s="8"/>
       <c r="F162" s="8"/>
       <c r="G162" s="8"/>
-      <c r="H162" s="8"/>
+      <c r="H162" s="7"/>
       <c r="I162" s="7"/>
       <c r="J162" s="4"/>
     </row>
-    <row r="163" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="4"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
-      <c r="E163" s="8"/>
-      <c r="F163" s="8"/>
-      <c r="G163" s="8"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
       <c r="J163" s="4"/>
     </row>
-    <row r="164" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="4"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
+    <row r="164" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A164" s="2"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
-      <c r="H164" s="8"/>
-      <c r="I164" s="8"/>
+      <c r="H164" s="7"/>
+      <c r="I164" s="7"/>
       <c r="J164" s="4"/>
     </row>
     <row r="165" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5397,23 +5487,23 @@
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
+      <c r="E165" s="8"/>
+      <c r="F165" s="8"/>
+      <c r="G165" s="8"/>
       <c r="H165" s="8"/>
-      <c r="I165" s="8"/>
+      <c r="I165" s="7"/>
       <c r="J165" s="4"/>
     </row>
     <row r="166" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4"/>
-      <c r="B166" s="8"/>
-      <c r="C166" s="8"/>
-      <c r="D166" s="8"/>
-      <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
-      <c r="G166" s="7"/>
+      <c r="B166" s="7"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="8"/>
+      <c r="F166" s="8"/>
+      <c r="G166" s="8"/>
       <c r="H166" s="8"/>
-      <c r="I166" s="8"/>
+      <c r="I166" s="7"/>
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5421,9 +5511,9 @@
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
-      <c r="F167" s="7"/>
-      <c r="G167" s="7"/>
+      <c r="E167" s="8"/>
+      <c r="F167" s="8"/>
+      <c r="G167" s="8"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
       <c r="J167" s="4"/>
@@ -5436,8 +5526,8 @@
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
-      <c r="H168" s="7"/>
-      <c r="I168" s="7"/>
+      <c r="H168" s="8"/>
+      <c r="I168" s="8"/>
       <c r="J168" s="4"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5448,20 +5538,20 @@
       <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
-      <c r="H169" s="7"/>
-      <c r="I169" s="7"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8"/>
       <c r="J169" s="4"/>
     </row>
     <row r="170" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
-      <c r="D170" s="7"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
       <c r="E170" s="7"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
-      <c r="H170" s="7"/>
-      <c r="I170" s="7"/>
+      <c r="H170" s="8"/>
+      <c r="I170" s="8"/>
       <c r="J170" s="4"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6534,50 +6624,50 @@
     </row>
     <row r="260" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="4"/>
-      <c r="B260" s="4"/>
-      <c r="C260" s="4"/>
-      <c r="D260" s="4"/>
-      <c r="E260" s="4"/>
-      <c r="F260" s="4"/>
-      <c r="G260" s="4"/>
-      <c r="H260" s="4"/>
-      <c r="I260" s="4"/>
+      <c r="B260" s="7"/>
+      <c r="C260" s="7"/>
+      <c r="D260" s="7"/>
+      <c r="E260" s="7"/>
+      <c r="F260" s="7"/>
+      <c r="G260" s="7"/>
+      <c r="H260" s="7"/>
+      <c r="I260" s="7"/>
       <c r="J260" s="4"/>
     </row>
     <row r="261" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="4"/>
-      <c r="B261" s="4"/>
-      <c r="C261" s="4"/>
-      <c r="D261" s="4"/>
-      <c r="E261" s="4"/>
-      <c r="F261" s="4"/>
-      <c r="G261" s="4"/>
-      <c r="H261" s="4"/>
-      <c r="I261" s="4"/>
+      <c r="B261" s="7"/>
+      <c r="C261" s="7"/>
+      <c r="D261" s="7"/>
+      <c r="E261" s="7"/>
+      <c r="F261" s="7"/>
+      <c r="G261" s="7"/>
+      <c r="H261" s="7"/>
+      <c r="I261" s="7"/>
       <c r="J261" s="4"/>
     </row>
     <row r="262" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="4"/>
-      <c r="B262" s="4"/>
-      <c r="C262" s="4"/>
-      <c r="D262" s="4"/>
-      <c r="E262" s="4"/>
-      <c r="F262" s="4"/>
-      <c r="G262" s="4"/>
-      <c r="H262" s="4"/>
-      <c r="I262" s="4"/>
+      <c r="B262" s="7"/>
+      <c r="C262" s="7"/>
+      <c r="D262" s="7"/>
+      <c r="E262" s="7"/>
+      <c r="F262" s="7"/>
+      <c r="G262" s="7"/>
+      <c r="H262" s="7"/>
+      <c r="I262" s="7"/>
       <c r="J262" s="4"/>
     </row>
     <row r="263" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="4"/>
-      <c r="B263" s="4"/>
-      <c r="C263" s="4"/>
-      <c r="D263" s="4"/>
-      <c r="E263" s="4"/>
-      <c r="F263" s="4"/>
-      <c r="G263" s="4"/>
-      <c r="H263" s="4"/>
-      <c r="I263" s="4"/>
+      <c r="B263" s="7"/>
+      <c r="C263" s="7"/>
+      <c r="D263" s="7"/>
+      <c r="E263" s="7"/>
+      <c r="F263" s="7"/>
+      <c r="G263" s="7"/>
+      <c r="H263" s="7"/>
+      <c r="I263" s="7"/>
       <c r="J263" s="4"/>
     </row>
     <row r="264" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7250,6 +7340,7 @@
       <c r="G319" s="4"/>
       <c r="H319" s="4"/>
       <c r="I319" s="4"/>
+      <c r="J319" s="4"/>
     </row>
     <row r="320" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="4"/>
@@ -7261,8 +7352,9 @@
       <c r="G320" s="4"/>
       <c r="H320" s="4"/>
       <c r="I320" s="4"/>
-    </row>
-    <row r="321" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J320" s="4"/>
+    </row>
+    <row r="321" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="4"/>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -7272,8 +7364,9 @@
       <c r="G321" s="4"/>
       <c r="H321" s="4"/>
       <c r="I321" s="4"/>
-    </row>
-    <row r="322" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J321" s="4"/>
+    </row>
+    <row r="322" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="4"/>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -7283,8 +7376,9 @@
       <c r="G322" s="4"/>
       <c r="H322" s="4"/>
       <c r="I322" s="4"/>
-    </row>
-    <row r="323" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J322" s="4"/>
+    </row>
+    <row r="323" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="4"/>
       <c r="B323" s="4"/>
       <c r="C323" s="4"/>
@@ -7295,7 +7389,7 @@
       <c r="H323" s="4"/>
       <c r="I323" s="4"/>
     </row>
-    <row r="324" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="4"/>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -7306,7 +7400,7 @@
       <c r="H324" s="4"/>
       <c r="I324" s="4"/>
     </row>
-    <row r="325" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="4"/>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -7317,7 +7411,7 @@
       <c r="H325" s="4"/>
       <c r="I325" s="4"/>
     </row>
-    <row r="326" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="4"/>
       <c r="B326" s="4"/>
       <c r="C326" s="4"/>
@@ -7328,7 +7422,7 @@
       <c r="H326" s="4"/>
       <c r="I326" s="4"/>
     </row>
-    <row r="327" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="4"/>
       <c r="B327" s="4"/>
       <c r="C327" s="4"/>
@@ -7339,7 +7433,7 @@
       <c r="H327" s="4"/>
       <c r="I327" s="4"/>
     </row>
-    <row r="328" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="4"/>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -7350,7 +7444,7 @@
       <c r="H328" s="4"/>
       <c r="I328" s="4"/>
     </row>
-    <row r="329" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="4"/>
       <c r="B329" s="4"/>
       <c r="C329" s="4"/>
@@ -7361,7 +7455,7 @@
       <c r="H329" s="4"/>
       <c r="I329" s="4"/>
     </row>
-    <row r="330" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="4"/>
       <c r="B330" s="4"/>
       <c r="C330" s="4"/>
@@ -7372,7 +7466,7 @@
       <c r="H330" s="4"/>
       <c r="I330" s="4"/>
     </row>
-    <row r="331" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="4"/>
       <c r="B331" s="4"/>
       <c r="C331" s="4"/>
@@ -7383,7 +7477,7 @@
       <c r="H331" s="4"/>
       <c r="I331" s="4"/>
     </row>
-    <row r="332" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="4"/>
       <c r="B332" s="4"/>
       <c r="C332" s="4"/>
@@ -7394,7 +7488,7 @@
       <c r="H332" s="4"/>
       <c r="I332" s="4"/>
     </row>
-    <row r="333" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="4"/>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -7405,7 +7499,7 @@
       <c r="H333" s="4"/>
       <c r="I333" s="4"/>
     </row>
-    <row r="334" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="4"/>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -7416,7 +7510,7 @@
       <c r="H334" s="4"/>
       <c r="I334" s="4"/>
     </row>
-    <row r="335" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="4"/>
       <c r="B335" s="4"/>
       <c r="C335" s="4"/>
@@ -7427,119 +7521,135 @@
       <c r="H335" s="4"/>
       <c r="I335" s="4"/>
     </row>
-    <row r="336" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="4"/>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
       <c r="D336" s="4"/>
       <c r="E336" s="4"/>
-    </row>
-    <row r="337" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F336" s="4"/>
+      <c r="G336" s="4"/>
+      <c r="H336" s="4"/>
+      <c r="I336" s="4"/>
+    </row>
+    <row r="337" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="4"/>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
       <c r="D337" s="4"/>
       <c r="E337" s="4"/>
-    </row>
-    <row r="338" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F337" s="4"/>
+      <c r="G337" s="4"/>
+      <c r="H337" s="4"/>
+      <c r="I337" s="4"/>
+    </row>
+    <row r="338" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="4"/>
       <c r="B338" s="4"/>
       <c r="C338" s="4"/>
       <c r="D338" s="4"/>
       <c r="E338" s="4"/>
-    </row>
-    <row r="339" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F338" s="4"/>
+      <c r="G338" s="4"/>
+      <c r="H338" s="4"/>
+      <c r="I338" s="4"/>
+    </row>
+    <row r="339" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="4"/>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
       <c r="D339" s="4"/>
       <c r="E339" s="4"/>
-    </row>
-    <row r="340" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F339" s="4"/>
+      <c r="G339" s="4"/>
+      <c r="H339" s="4"/>
+      <c r="I339" s="4"/>
+    </row>
+    <row r="340" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="4"/>
       <c r="B340" s="4"/>
       <c r="C340" s="4"/>
       <c r="D340" s="4"/>
       <c r="E340" s="4"/>
     </row>
-    <row r="341" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
       <c r="D341" s="4"/>
       <c r="E341" s="4"/>
     </row>
-    <row r="342" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="B342" s="4"/>
       <c r="C342" s="4"/>
       <c r="D342" s="4"/>
       <c r="E342" s="4"/>
     </row>
-    <row r="343" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="4"/>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
       <c r="D343" s="4"/>
       <c r="E343" s="4"/>
     </row>
-    <row r="344" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="4"/>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
       <c r="D344" s="4"/>
       <c r="E344" s="4"/>
     </row>
-    <row r="345" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="4"/>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
       <c r="D345" s="4"/>
       <c r="E345" s="4"/>
     </row>
-    <row r="346" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="4"/>
       <c r="B346" s="4"/>
       <c r="C346" s="4"/>
       <c r="D346" s="4"/>
       <c r="E346" s="4"/>
     </row>
-    <row r="347" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="4"/>
       <c r="B347" s="4"/>
       <c r="C347" s="4"/>
       <c r="D347" s="4"/>
       <c r="E347" s="4"/>
     </row>
-    <row r="348" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="4"/>
       <c r="B348" s="4"/>
       <c r="C348" s="4"/>
       <c r="D348" s="4"/>
       <c r="E348" s="4"/>
     </row>
-    <row r="349" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="4"/>
       <c r="B349" s="4"/>
       <c r="C349" s="4"/>
       <c r="D349" s="4"/>
       <c r="E349" s="4"/>
     </row>
-    <row r="350" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="4"/>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
       <c r="D350" s="4"/>
       <c r="E350" s="4"/>
     </row>
-    <row r="351" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="4"/>
       <c r="B351" s="4"/>
       <c r="C351" s="4"/>
       <c r="D351" s="4"/>
       <c r="E351" s="4"/>
     </row>
-    <row r="352" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="4"/>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -8581,7 +8691,6 @@
       <c r="C500" s="4"/>
       <c r="D500" s="4"/>
       <c r="E500" s="4"/>
-      <c r="I500" s="4"/>
     </row>
     <row r="501" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A501" s="4"/>
@@ -8610,6 +8719,7 @@
       <c r="C504" s="4"/>
       <c r="D504" s="4"/>
       <c r="E504" s="4"/>
+      <c r="I504" s="4"/>
     </row>
     <row r="505" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A505" s="4"/>
@@ -8940,8 +9050,106 @@
       <c r="D551" s="4"/>
       <c r="E551" s="4"/>
     </row>
+    <row r="552" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A552" s="4"/>
+      <c r="B552" s="4"/>
+      <c r="C552" s="4"/>
+      <c r="D552" s="4"/>
+      <c r="E552" s="4"/>
+    </row>
+    <row r="553" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A553" s="4"/>
+      <c r="B553" s="4"/>
+      <c r="C553" s="4"/>
+      <c r="D553" s="4"/>
+      <c r="E553" s="4"/>
+    </row>
+    <row r="554" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A554" s="4"/>
+      <c r="B554" s="4"/>
+      <c r="C554" s="4"/>
+      <c r="D554" s="4"/>
+      <c r="E554" s="4"/>
+    </row>
+    <row r="555" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A555" s="4"/>
+      <c r="B555" s="4"/>
+      <c r="C555" s="4"/>
+      <c r="D555" s="4"/>
+      <c r="E555" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="86">
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="D77:D79"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="F77:F79"/>
+    <mergeCell ref="G77:G79"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="G67:G69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="G73:G76"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="D73:D76"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="D6:D15"/>
+    <mergeCell ref="E6:E15"/>
+    <mergeCell ref="G6:G15"/>
+    <mergeCell ref="F6:F15"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="D70:D72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="G56:G59"/>
+    <mergeCell ref="F56:F59"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="G63:G66"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C39:C50"/>
+    <mergeCell ref="B39:B50"/>
+    <mergeCell ref="C3:C15"/>
+    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="C51:C62"/>
+    <mergeCell ref="B3:B15"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="B16:B26"/>
+    <mergeCell ref="B51:B62"/>
+    <mergeCell ref="G51:G55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="D60:D62"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:F5"/>
@@ -8958,72 +9166,6 @@
     <mergeCell ref="E22:E26"/>
     <mergeCell ref="F22:F26"/>
     <mergeCell ref="G22:G26"/>
-    <mergeCell ref="G51:G55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="C39:C50"/>
-    <mergeCell ref="B39:B50"/>
-    <mergeCell ref="C3:C15"/>
-    <mergeCell ref="C16:C26"/>
-    <mergeCell ref="C51:C58"/>
-    <mergeCell ref="B3:B15"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="B16:B26"/>
-    <mergeCell ref="B51:B58"/>
-    <mergeCell ref="G59:G62"/>
-    <mergeCell ref="F59:F62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="F45:F50"/>
-    <mergeCell ref="G45:G50"/>
-    <mergeCell ref="F66:F68"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="D6:D15"/>
-    <mergeCell ref="E6:E15"/>
-    <mergeCell ref="G6:G15"/>
-    <mergeCell ref="F6:F15"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="F33:F38"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G73:G75"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="G63:G65"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="E63:E65"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="G69:G72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="G66:G68"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="C73:C75"/>
-    <mergeCell ref="D73:D75"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="F73:F75"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9048,111 +9190,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="46" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="49" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="84"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="85"/>
+      <c r="D6" s="50"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="49" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="49"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="85"/>
+      <c r="D9" s="50"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="85"/>
+      <c r="D10" s="50"/>
     </row>
     <row r="11" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="85"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="12" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="85"/>
+      <c r="D12" s="50"/>
     </row>
     <row r="13" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
@@ -9163,7 +9305,7 @@
       <c r="C14" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="79"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9227,7 +9369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -9239,117 +9381,117 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="57" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="58" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="58" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="58" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="58" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="58" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="D8" s="58" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="58" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="91" t="s">
+      <c r="C10" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="59" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="80"/>
+      <c r="F18" s="45"/>
     </row>
     <row r="19" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F19" s="80"/>
+      <c r="F19" s="45"/>
     </row>
     <row r="20" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="80"/>
-      <c r="F20" s="80"/>
+      <c r="C20" s="45"/>
+      <c r="F20" s="45"/>
     </row>
     <row r="21" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="80"/>
-      <c r="F21" s="80"/>
+      <c r="C21" s="45"/>
+      <c r="F21" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>